<commit_message>
Differentiate between 3D and 1D.
</commit_message>
<xml_diff>
--- a/Chimera/Chimera_1D/gradient_calc.xlsx
+++ b/Chimera/Chimera_1D/gradient_calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/Graduate Research/Chimera/Chimera/Chimera_1D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA38C2AB-BF30-2949-B4AC-3BCC3B4998BA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D368F53-9A67-4441-B38E-D6CD1F2FC1A3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="15800" windowHeight="16480" xr2:uid="{8C3FC4A1-B589-6044-A34C-DD3123E36A55}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,7 +445,7 @@
         <v>20</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>40</v>
@@ -459,7 +459,7 @@
       </c>
       <c r="H2">
         <f>B2+((G2/C2)*D2)</f>
-        <v>2499.8000000000002</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -468,14 +468,15 @@
       </c>
       <c r="B3">
         <f>H2</f>
-        <v>2499.8000000000002</v>
+        <v>4499</v>
       </c>
       <c r="C3">
         <f>C2</f>
         <v>20</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <f>D2</f>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>50040</v>
@@ -489,7 +490,7 @@
       </c>
       <c r="H3">
         <f>B3+((G3/C3)*D3)</f>
-        <v>2999</v>
+        <v>6995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>